<commit_message>
Fix: Build the DT to be used as Queue
</commit_message>
<xml_diff>
--- a/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
+++ b/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\Customer_Issue_Resolution_Bot\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0632D4A3-10B4-4648-B54B-DCC6CA5B5955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F7D2C6-7147-435E-9FEF-DD6225A2EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{B9E339D8-5102-4FDB-A5C5-07ECB7712C3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B9E339D8-5102-4FDB-A5C5-07ECB7712C3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Issue Log" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>AI Genereated Response</t>
   </si>
   <si>
-    <t>Staus (Resolved/Unresolved)</t>
-  </si>
-  <si>
     <t>Date of Resolution</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>Escalated (Yes/No)</t>
+  </si>
+  <si>
+    <t>Email Body</t>
+  </si>
+  <si>
+    <t>Customer Email</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Email Subject</t>
   </si>
 </sst>
 </file>
@@ -485,40 +494,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB5E927-5256-49CB-B63F-9076C9E9FC05}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -547,25 +564,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDBAA3B-35A9-4F52-8920-39167EE27CE3}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -593,22 +610,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -636,22 +653,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Updated the Get Transaction flow
</commit_message>
<xml_diff>
--- a/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
+++ b/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\Customer_Issue_Resolution_Bot\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F7D2C6-7147-435E-9FEF-DD6225A2EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FABE48-38E8-4883-A147-1FF1086239D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B9E339D8-5102-4FDB-A5C5-07ECB7712C3D}"/>
   </bookViews>
@@ -39,38 +39,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>Customer Email</t>
+  </si>
+  <si>
+    <t>Email Subject</t>
+  </si>
+  <si>
+    <t>Email Body</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>AI Genereated Response</t>
+  </si>
+  <si>
+    <t>Issue Category</t>
+  </si>
+  <si>
+    <t>Date of Resolution</t>
+  </si>
+  <si>
+    <t>10/15/2024 08:10:28</t>
+  </si>
+  <si>
+    <t>kiongobob@gmail.com</t>
+  </si>
+  <si>
+    <t>Fwd: Question About Your Service Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:35 AM
+Subject: Fwd: Question About Your Service Hours
+To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:33 AM
+Subject: Question About Your Service Hours
+To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
+Dear Team,
+I was wondering if you could confirm your operating hours during the weekend. I would like to visit your store, but I want to make sure it’s open before I plan my trip.
+Thank you in advance!
+Best,
+Bob
+</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
+  <si>
+    <t>Fwd: New account configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:35 AM
+Subject: Fwd: New account configuration
+To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:31 AM
+Subject: New account configuration
+To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
+Hello, could you please provide a link to the documentation or other resources on how to configure a new admin account to configure multiple users?
+regards</t>
+  </si>
+  <si>
+    <t>Fwd: Trouble with account payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:35 AM
+Subject: Fwd: Trouble with account payment
+To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:29 AM
+Subject: Trouble with account payment
+To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
+My payment is failing, kindly assist.
+Regards.</t>
+  </si>
+  <si>
+    <t>Fwd: Ethernet cable not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Tue, Oct 15, 2024 at 5:35 AM
+Subject: Fwd: Ethernet cable not working
+To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
+---------- Forwarded message ---------
+From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
+Date: Mon, Oct 14, 2024 at 12:38 PM
+Subject: Ethernet cable not working
+To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
+Hello, I hope this email finds you well. My ethernet cable is not working as expected, kindly assist.
+Regards,
+Bob.</t>
+  </si>
+  <si>
+    <t>Date Escalated</t>
+  </si>
+  <si>
     <t>Customer email</t>
   </si>
   <si>
-    <t>AI Genereated Response</t>
-  </si>
-  <si>
-    <t>Date of Resolution</t>
-  </si>
-  <si>
-    <t>Issue Category</t>
-  </si>
-  <si>
-    <t>Date Escalated</t>
-  </si>
-  <si>
     <t>Issue Description (Email body)</t>
   </si>
   <si>
+    <t xml:space="preserve">AI Attempts </t>
+  </si>
+  <si>
     <t>Assigned Agent</t>
   </si>
   <si>
     <t>Status (Pending/Resolved</t>
   </si>
   <si>
-    <t xml:space="preserve">AI Attempts </t>
-  </si>
-  <si>
     <t>Number of Issues Handled</t>
   </si>
   <si>
@@ -102,18 +200,6 @@
   </si>
   <si>
     <t>Escalated (Yes/No)</t>
-  </si>
-  <si>
-    <t>Email Body</t>
-  </si>
-  <si>
-    <t>Customer Email</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Email Subject</t>
   </si>
 </sst>
 </file>
@@ -157,9 +243,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,48 +583,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB5E927-5256-49CB-B63F-9076C9E9FC05}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -562,27 +719,27 @@
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -608,24 +765,24 @@
     <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -651,24 +808,24 @@
     <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Updated the DT from Get Transaction State
</commit_message>
<xml_diff>
--- a/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
+++ b/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\Customer_Issue_Resolution_Bot\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FABE48-38E8-4883-A147-1FF1086239D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30328FB-C816-4266-B17D-D244127F68D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B9E339D8-5102-4FDB-A5C5-07ECB7712C3D}"/>
   </bookViews>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Customer Email</t>
-  </si>
-  <si>
     <t>Email Subject</t>
   </si>
   <si>
@@ -63,92 +60,6 @@
   </si>
   <si>
     <t>Date of Resolution</t>
-  </si>
-  <si>
-    <t>10/15/2024 08:10:28</t>
-  </si>
-  <si>
-    <t>kiongobob@gmail.com</t>
-  </si>
-  <si>
-    <t>Fwd: Question About Your Service Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:35 AM
-Subject: Fwd: Question About Your Service Hours
-To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:33 AM
-Subject: Question About Your Service Hours
-To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
-Dear Team,
-I was wondering if you could confirm your operating hours during the weekend. I would like to visit your store, but I want to make sure it’s open before I plan my trip.
-Thank you in advance!
-Best,
-Bob
-</t>
-  </si>
-  <si>
-    <t>Unresolved</t>
-  </si>
-  <si>
-    <t>Fwd: New account configuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:35 AM
-Subject: Fwd: New account configuration
-To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:31 AM
-Subject: New account configuration
-To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
-Hello, could you please provide a link to the documentation or other resources on how to configure a new admin account to configure multiple users?
-regards</t>
-  </si>
-  <si>
-    <t>Fwd: Trouble with account payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:35 AM
-Subject: Fwd: Trouble with account payment
-To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:29 AM
-Subject: Trouble with account payment
-To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
-My payment is failing, kindly assist.
-Regards.</t>
-  </si>
-  <si>
-    <t>Fwd: Ethernet cable not working</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Tue, Oct 15, 2024 at 5:35 AM
-Subject: Fwd: Ethernet cable not working
-To: &lt;mutuahfredrick@gmail.com &lt;mailto:mutuahfredrick@gmail.com&gt; &gt;
----------- Forwarded message ---------
-From: Bob Kiongo &lt;kiongobob@gmail.com &lt;mailto:kiongobob@gmail.com&gt; &gt;
-Date: Mon, Oct 14, 2024 at 12:38 PM
-Subject: Ethernet cable not working
-To: &lt;brian.njogu@griffinglobaltech.com &lt;mailto:brian.njogu@griffinglobaltech.com&gt; &gt;
-Hello, I hope this email finds you well. My ethernet cable is not working as expected, kindly assist.
-Regards,
-Bob.</t>
   </si>
   <si>
     <t>Date Escalated</t>
@@ -586,16 +497,16 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -605,95 +516,37 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -721,25 +574,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -767,22 +620,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -810,22 +663,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Implemented logging back to Customer Excel
- Implemented updating the excel sheet columns after mail is sent
- Improved the logging messaeges
- Cleaned the code
</commit_message>
<xml_diff>
--- a/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
+++ b/Data/Output/Customer_Issue_Resolutionxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\Customer_Issue_Resolution_Bot\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A14E361-9ACF-4175-8A55-E8C21A0B173D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11E7911-35D2-41DA-981E-312F7BC71959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B9E339D8-5102-4FDB-A5C5-07ECB7712C3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -62,7 +62,7 @@
     <t>Date of Resolution</t>
   </si>
   <si>
-    <t>10/15/2024 14:12:53</t>
+    <t>10/15/2024 20:50:43</t>
   </si>
   <si>
     <t>kiongobob@gmail.com</t>
@@ -79,10 +79,24 @@
 </t>
   </si>
   <si>
-    <t>Unresolved</t>
-  </si>
-  <si>
-    <t>10/15/2024 14:12:54</t>
+    <t>Solution Mailed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Reply to the customer acknowledging the issue and thanking them for bringing it to your attention.
+2. Review the invoice (No: 123456) to verify the extra charge and compare it with the services the customer has subscribed to.
+3. If the charge is indeed incorrect, adjust the billing accordingly and provide the customer with an updated invoice reflecting the correct amount.
+4. Inform the customer of the correction made and apologize for any inconvenience caused by the billing error.
+Would you like any assistance in drafting a response email to the customer?</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>10/15/2024 20:51:20</t>
+  </si>
+  <si>
+    <t>10/15/2024 20:50:44</t>
   </si>
   <si>
     <t>New account configuration</t>
@@ -98,9 +112,6 @@
     <t xml:space="preserve">My payment is failing, kindly assist.
 Regards.
 </t>
-  </si>
-  <si>
-    <t>10/15/2024 14:12:55</t>
   </si>
   <si>
     <t>Ethernet cable not working</t>
@@ -119,6 +130,9 @@
 Thanks in advance!
 Best,
 </t>
+  </si>
+  <si>
+    <t>10/15/2024 20:50:45</t>
   </si>
   <si>
     <t>Request to Cancel My Subscription</t>
@@ -130,9 +144,6 @@
 Regards,
 Peter Combs
 </t>
-  </si>
-  <si>
-    <t>10/15/2024 14:12:56</t>
   </si>
   <si>
     <t>Data Privacy Request - Access to My Personal Information</t>
@@ -220,7 +231,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,23 +570,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB5E927-5256-49CB-B63F-9076C9E9FC05}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="68.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="16384" width="28.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -599,157 +605,238 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="360" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>